<commit_message>
Form11 and Dep Report are styled
</commit_message>
<xml_diff>
--- a/Planner/Planner/App_Data/Form11.xlsx
+++ b/Planner/Planner/App_Data/Form11.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>ПІБ</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Вихідні дані</t>
   </si>
@@ -30,9 +27,6 @@
     <t>дата видання</t>
   </si>
   <si>
-    <t>назва публікації</t>
-  </si>
-  <si>
     <t>кол.друк. листов</t>
   </si>
   <si>
@@ -45,16 +39,19 @@
     <t>Модернизация: путь в будущее</t>
   </si>
   <si>
-    <t>Іванов І.І.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Економіка розвитку, 2015.  -№3. - С. 21-36. </t>
   </si>
   <si>
-    <t>тип*</t>
-  </si>
-  <si>
     <t xml:space="preserve">Наукові публікації на період </t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>тип</t>
+  </si>
+  <si>
+    <t>Назва публікації</t>
   </si>
 </sst>
 </file>
@@ -504,63 +501,62 @@
   <dimension ref="A2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C2" s="14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4">
-        <v>429</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <v>42112</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="F4" s="7">
         <v>0.44</v>

</xml_diff>